<commit_message>
Fixes to air to air combat hit allocation
Signed-off-by: NB-MikeRichardson <mike.richardson@northernblock.io>
</commit_message>
<xml_diff>
--- a/resources/ES1PearlHarbor.xlsx
+++ b/resources/ES1PearlHarbor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pacific War\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\new\pacificwar\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C241E5-2CC3-42AA-A26C-B324BA1DD36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{72527C8B-B5F6-4670-832C-FC069318334E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{01B5032C-F34A-48B0-92F4-FB0450D7D458}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="es1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -715,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FB452B-8972-47D9-A54E-7D13DFEF60FA}">
   <dimension ref="A1:Z44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added code for resolving Flak
Signed-off-by: NB-MikeRichardson <mike.richardson@northernblock.io>
</commit_message>
<xml_diff>
--- a/resources/ES1PearlHarbor.xlsx
+++ b/resources/ES1PearlHarbor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\new\pacificwar\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72527C8B-B5F6-4670-832C-FC069318334E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5360F6DF-1573-4F2F-996E-7099815BB4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{01B5032C-F34A-48B0-92F4-FB0450D7D458}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="es1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -350,9 +349,6 @@
     <t>Hex</t>
   </si>
   <si>
-    <t>Pearl Harbor</t>
-  </si>
-  <si>
     <t>SubUnit</t>
   </si>
   <si>
@@ -360,6 +356,9 @@
   </si>
   <si>
     <t>CA6</t>
+  </si>
+  <si>
+    <t>Pearl Harbor Base</t>
   </si>
 </sst>
 </file>
@@ -716,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FB452B-8972-47D9-A54E-7D13DFEF60FA}">
   <dimension ref="A1:Z44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X12" sqref="X12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1652,12 +1651,12 @@
         <v>60</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G18" s="1">
         <v>18</v>
@@ -2040,7 +2039,7 @@
         <v>3</v>
       </c>
       <c r="F26" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
@@ -2091,7 +2090,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
@@ -2142,7 +2141,7 @@
         <v>2</v>
       </c>
       <c r="F28" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
@@ -2184,7 +2183,7 @@
         <v>2</v>
       </c>
       <c r="F29" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1" t="s">
@@ -2226,7 +2225,7 @@
         <v>2</v>
       </c>
       <c r="F30" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1" t="s">
@@ -2268,7 +2267,7 @@
         <v>2</v>
       </c>
       <c r="F31" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1" t="s">
@@ -2310,7 +2309,7 @@
         <v>2</v>
       </c>
       <c r="F32" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
@@ -2343,7 +2342,7 @@
         <v>60</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>82</v>
@@ -2352,7 +2351,7 @@
         <v>2</v>
       </c>
       <c r="F33" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1" t="s">
@@ -2385,7 +2384,7 @@
         <v>60</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>84</v>
@@ -2789,7 +2788,7 @@
         <v>60</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X44" s="1">
         <v>36</v>

</xml_diff>